<commit_message>
Update Risk and Issue
</commit_message>
<xml_diff>
--- a/7. Risk Management/BSS_RiskAndIssueList_V1.1.xlsx
+++ b/7. Risk Management/BSS_RiskAndIssueList_V1.1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19560" windowHeight="9405" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19560" windowHeight="9405" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Dash Board" sheetId="4" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="96">
   <si>
     <t>ID</t>
   </si>
@@ -310,6 +310,9 @@
   </si>
   <si>
     <t>Resources is turn over</t>
+  </si>
+  <si>
+    <t>15/1/2017</t>
   </si>
 </sst>
 </file>
@@ -1672,7 +1675,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1896,7 +1898,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:solidFill>
@@ -2033,7 +2034,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2278,10 +2278,10 @@
                   <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>7</c:v>
@@ -2317,7 +2317,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:solidFill>
@@ -2446,7 +2445,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2612,11 +2610,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="65"/>
-        <c:axId val="72508544"/>
-        <c:axId val="72519680"/>
+        <c:axId val="60577664"/>
+        <c:axId val="60596992"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="72508544"/>
+        <c:axId val="60577664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2659,7 +2657,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="72519680"/>
+        <c:crossAx val="60596992"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2667,7 +2665,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="72519680"/>
+        <c:axId val="60596992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2703,7 +2701,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="72508544"/>
+        <c:crossAx val="60577664"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2851,7 +2849,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2999,10 +2996,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>5</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3035,7 +3032,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:solidFill>
@@ -3784,7 +3780,7 @@
         <xdr:cNvPr id="4" name="Chart 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CE0ED5F5-A0D8-4C7F-A05B-AF65D92FB984}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{CE0ED5F5-A0D8-4C7F-A05B-AF65D92FB984}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3822,7 +3818,7 @@
         <xdr:cNvPr id="5" name="Chart 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DF3CB91A-BF33-47BF-86B2-5302FF3E0625}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{DF3CB91A-BF33-47BF-86B2-5302FF3E0625}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3860,7 +3856,7 @@
         <xdr:cNvPr id="6" name="Chart 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{745C757D-EEA0-4E8F-A7DF-4917898F0AF6}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{745C757D-EEA0-4E8F-A7DF-4917898F0AF6}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3896,7 +3892,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D8EAB6BE-AD1C-4008-B2AD-2A535C15335C}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{D8EAB6BE-AD1C-4008-B2AD-2A535C15335C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4215,7 +4211,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -4316,7 +4312,7 @@
       </c>
       <c r="C8" s="26">
         <f>COUNTIFS('Risk List'!$E$6:$E$32,"In Progress",'Risk List'!$K$6:$K$32,"High")</f>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D8" s="26">
         <f>COUNTIFS('Risk List'!$E$6:$E$32,"In Progress",'Risk List'!$K$6:$K$32,"Medium")</f>
@@ -4328,11 +4324,11 @@
       </c>
       <c r="F8" s="27">
         <f>SUM(C8:E8)</f>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="G8" s="28">
         <f>F8/F11</f>
-        <v>0.20833333333333334</v>
+        <v>0.125</v>
       </c>
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.25">
@@ -4341,7 +4337,7 @@
       </c>
       <c r="C9" s="26">
         <f>COUNTIFS('Risk List'!$E$6:$E$32,"Closed",'Risk List'!$K$6:$K$32,"High")</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D9" s="26">
         <f>COUNTIFS('Risk List'!$E$6:$E$32,"Closed",'Risk List'!$K$6:$K$32,"Medium")</f>
@@ -4353,11 +4349,11 @@
       </c>
       <c r="F9" s="27">
         <f>SUM(C9:E9)</f>
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="G9" s="41">
         <f>F9/F11</f>
-        <v>0.20833333333333334</v>
+        <v>0.29166666666666669</v>
       </c>
     </row>
     <row r="10" spans="2:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -4455,7 +4451,7 @@
       </c>
       <c r="F15" s="26">
         <f>COUNTIF(Table13[Actual Status], "Active")</f>
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="16" spans="2:7" x14ac:dyDescent="0.25">
@@ -4471,7 +4467,7 @@
       </c>
       <c r="F16" s="26">
         <f>COUNTIF(Table13[Actual Status],"Fixed")</f>
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.25">
@@ -4546,8 +4542,8 @@
   </sheetPr>
   <dimension ref="A1:AB33"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="10.5" x14ac:dyDescent="0.15"/>
@@ -4693,7 +4689,7 @@
         <v>16</v>
       </c>
       <c r="E7" s="63" t="s">
-        <v>47</v>
+        <v>9</v>
       </c>
       <c r="F7" s="60">
         <v>42653</v>
@@ -5139,7 +5135,7 @@
         <v>13</v>
       </c>
       <c r="E18" s="59" t="s">
-        <v>47</v>
+        <v>9</v>
       </c>
       <c r="F18" s="60">
         <v>42681</v>
@@ -5725,8 +5721,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:I16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5802,12 +5798,14 @@
         <v>16</v>
       </c>
       <c r="E5" s="50" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F5" s="22" t="s">
         <v>82</v>
       </c>
-      <c r="G5" s="22"/>
+      <c r="G5" s="22">
+        <v>42738</v>
+      </c>
       <c r="H5" s="17" t="s">
         <v>3</v>
       </c>
@@ -5977,12 +5975,14 @@
         <v>14</v>
       </c>
       <c r="E12" s="16" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F12" s="22" t="s">
         <v>87</v>
       </c>
-      <c r="G12" s="22"/>
+      <c r="G12" s="22">
+        <v>42738</v>
+      </c>
       <c r="H12" s="17" t="s">
         <v>3</v>
       </c>
@@ -6003,10 +6003,10 @@
         <v>70</v>
       </c>
       <c r="F13" s="23" t="s">
-        <v>87</v>
+        <v>95</v>
       </c>
       <c r="G13" s="22">
-        <v>42738</v>
+        <v>42737</v>
       </c>
       <c r="H13" s="17" t="s">
         <v>2</v>

</xml_diff>